<commit_message>
added send email logic
</commit_message>
<xml_diff>
--- a/Master File.xlsx
+++ b/Master File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spatel\Documents\UiPath\Test process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29F0C8D-D993-4245-8BEB-097C26057445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDB5837-C440-459A-BC3E-CE555DD913C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -551,7 +551,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="A1:XFD1048576"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,20 +565,20 @@
     <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -686,6 +686,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>